<commit_message>
Update to project report + task list
</commit_message>
<xml_diff>
--- a/WDD_project_task_list.xlsx
+++ b/WDD_project_task_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27203"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oisin\Documents\WDD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EThornbury\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B7DC18C-A9CD-4E12-B01F-7531D135D85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7C39091-056F-4ED6-9D0A-1CF6424899FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="2796" windowWidth="17280" windowHeight="9960" xr2:uid="{CC4871A7-87E9-400E-8844-9811E13AA789}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{CC4871A7-87E9-400E-8844-9811E13AA789}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,65 +20,79 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
+  <si>
+    <t>WDD_Project_2023</t>
+  </si>
   <si>
     <t>Done Y/N?</t>
-  </si>
-  <si>
-    <t>Week</t>
-  </si>
-  <si>
-    <t>Goals for this week</t>
-  </si>
-  <si>
-    <t>week 8</t>
-  </si>
-  <si>
-    <t>read brief &amp; be familiar with it</t>
-  </si>
-  <si>
-    <t>week 9</t>
-  </si>
-  <si>
-    <t>week 10</t>
-  </si>
-  <si>
-    <t>week 11</t>
-  </si>
-  <si>
-    <t>week 12</t>
-  </si>
-  <si>
-    <t>Submission</t>
   </si>
   <si>
     <t>Team 
 Member</t>
   </si>
   <si>
-    <t>WDD_Project_2023</t>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Goals for this week</t>
+  </si>
+  <si>
+    <t>week 8</t>
+  </si>
+  <si>
+    <t>read brief &amp; be familiar with it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y </t>
   </si>
   <si>
     <t>brainstorm with group - what is website like</t>
   </si>
   <si>
+    <t>Christian, Oisin, Antoine</t>
+  </si>
+  <si>
     <t>team member strengths and weaknesses</t>
   </si>
   <si>
     <t>1 person creates a shared folder and shares it!</t>
   </si>
   <si>
+    <t>Antoine</t>
+  </si>
+  <si>
     <t>my own wireframe</t>
   </si>
   <si>
+    <t>week 9</t>
+  </si>
+  <si>
     <t>use wireframe to code up page</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
     <t>think about class and id names so no-one overwrites anothers CSS!</t>
   </si>
   <si>
@@ -88,10 +102,25 @@
     <t>decide website content</t>
   </si>
   <si>
-    <t>SUNDAY 10th DEC 11pm</t>
-  </si>
-  <si>
-    <t>decide who does this</t>
+    <t>record who contributed - meeting and coding</t>
+  </si>
+  <si>
+    <t>Let Emer know if someone is out of contact</t>
+  </si>
+  <si>
+    <t>week 10</t>
+  </si>
+  <si>
+    <t>add your tasks and assign them to a team member</t>
+  </si>
+  <si>
+    <t>week 11</t>
+  </si>
+  <si>
+    <t>week 12</t>
+  </si>
+  <si>
+    <t>finish up code</t>
   </si>
   <si>
     <t>deploy website</t>
@@ -100,32 +129,56 @@
     <t>testing - functional testing, speed test</t>
   </si>
   <si>
-    <t>finish up code</t>
-  </si>
-  <si>
     <t>Write/record report</t>
   </si>
   <si>
-    <t>record who contributed - meeting and coding</t>
-  </si>
-  <si>
-    <t>Let Emer know if someone is out of contact</t>
-  </si>
-  <si>
-    <t>add your tasks and assign them to a team member</t>
-  </si>
-  <si>
-    <t>Yes</t>
+    <t>Only one css file - if possible for more marks</t>
+  </si>
+  <si>
+    <t>Testing menu links work</t>
+  </si>
+  <si>
+    <t>Images in a folder - at least 4</t>
+  </si>
+  <si>
+    <t>form - must have 5 fields, JS validation</t>
   </si>
   <si>
     <t>Oisin</t>
+  </si>
+  <si>
+    <t>Comments in HTML, CSS and JS</t>
+  </si>
+  <si>
+    <t>Make sure the author name is one each webpage</t>
+  </si>
+  <si>
+    <t>Christian, Oisin</t>
+  </si>
+  <si>
+    <t>Everyone has DOM manipulation on their own webpage</t>
+  </si>
+  <si>
+    <t>Create wireframe + sitemap + moodboard (hex codes, fonts, images - moodboard)</t>
+  </si>
+  <si>
+    <t>Document the planning (excel task sheet), optimisation of images, html validation, menu links + JS, responsiveness</t>
+  </si>
+  <si>
+    <t>Christian, Antoine</t>
+  </si>
+  <si>
+    <t>Submission</t>
+  </si>
+  <si>
+    <t>Sunday 10th dec 11pm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,283 +543,329 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A20EA6-9FE1-4F65-A2C0-41C46F4D1B7C}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="23.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="81.109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.6640625" style="3"/>
+    <col min="1" max="1" width="14.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="81.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="46.8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="46.5">
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="B24" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="B29" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="B32" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="B33" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="C33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="B34" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="C34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="B35" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B12" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" s="3" t="s">
+    </row>
+    <row r="36" spans="1:11">
+      <c r="B36" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B29" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B32" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B33" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B34" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A36" s="3" t="s">
+      <c r="D36" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="B37" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="B38" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="B39" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B37" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>30</v>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="B40" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="B41" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="B42" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="B43" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -776,6 +875,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009267F4E1BDB0BA4ABFCFBFE514C604C8" ma:contentTypeVersion="32" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61ddfe86c7f6991e5d8570e77096b500">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a400bed3-dd80-47b5-be8a-0e5cea58c044" xmlns:ns3="bf565209-2b21-4ee4-af8d-f3a2c0cda902" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f845289874843908626a75dec0325abb" ns2:_="" ns3:_="">
     <xsd:import namespace="a400bed3-dd80-47b5-be8a-0e5cea58c044"/>
@@ -1178,7 +1286,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <DefaultSectionNames xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
@@ -1230,55 +1338,14 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4A6CF24-95A3-4D7A-A7CF-B44ADA1363FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a400bed3-dd80-47b5-be8a-0e5cea58c044"/>
-    <ds:schemaRef ds:uri="bf565209-2b21-4ee4-af8d-f3a2c0cda902"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8144FC7C-9872-4D39-8984-1737A434D946}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45813AF1-8288-45E9-83B6-FF3A559347C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="bf565209-2b21-4ee4-af8d-f3a2c0cda902"/>
-    <ds:schemaRef ds:uri="a400bed3-dd80-47b5-be8a-0e5cea58c044"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4A6CF24-95A3-4D7A-A7CF-B44ADA1363FA}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8144FC7C-9872-4D39-8984-1737A434D946}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45813AF1-8288-45E9-83B6-FF3A559347C4}"/>
 </file>
</xml_diff>